<commit_message>
hours updated and video link
</commit_message>
<xml_diff>
--- a/proj4documentation/TimeAccounting_EECS448project4.xlsx
+++ b/proj4documentation/TimeAccounting_EECS448project4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katelynblackburn/Desktop/College/2021 Spring/EECS 448/Project3/EECS448_Project3/proj4documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Desktop\ku\junior spring\EECS 448Projects\FinalProject\EECS448_Project3\proj4documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358B6A27-B707-E845-A808-3CD097598C2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A7C6D8-25C3-4AC1-AD8F-2C1E1EF39469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="18060" windowHeight="10416" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,19 +731,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="2" max="9" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.19921875" customWidth="1"/>
+    <col min="2" max="9" width="7.69921875" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.69921875" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="26" width="7.6640625" customWidth="1"/>
+    <col min="14" max="26" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -787,7 +787,7 @@
       </c>
       <c r="S1" s="66">
         <f>R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13</f>
-        <v>2.2291666666666679</v>
+        <v>2.2916666666666679</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
@@ -1121,15 +1121,19 @@
       </c>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
+      <c r="L11" s="33">
+        <v>0.875</v>
+      </c>
+      <c r="M11" s="33">
+        <v>0.9375</v>
+      </c>
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="29"/>
       <c r="R11" s="23">
         <f t="shared" ref="R11:R16" si="0">(E11-D11)+(I11-H11)+(K11-J11)+(M11-L11)+(O11-N11)+(Q11-P11)</f>
-        <v>8.333333333333337E-2</v>
+        <v>0.14583333333333337</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="14.25" customHeight="1">
@@ -1261,7 +1265,7 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="L15" s="33">
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="33">
         <v>0.16666666666666666</v>
@@ -1276,7 +1280,7 @@
       <c r="Q15" s="19"/>
       <c r="R15" s="23">
         <f t="shared" si="0"/>
-        <v>1.09375</v>
+        <v>1.1770833333333333</v>
       </c>
       <c r="S15" s="36"/>
       <c r="T15" s="36"/>
@@ -1407,7 +1411,7 @@
       <c r="L25" s="53"/>
       <c r="M25" s="54">
         <f>(M3-L3)+(M4-L4)+(M5-L5)+(M6-L6)+(M7-L7)+(M8-L8)+(M9-L9)+(M10-L10)+(M11-L11)+(M12-L12)+(M13-L13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)+(E14-D14)+(E15-D15)+(E16-D16)+(M14-L14)+(M15-L15)+(M16-L16)</f>
-        <v>0.71111111111111081</v>
+        <v>0.85694444444444418</v>
       </c>
       <c r="Q25" s="35"/>
       <c r="R25" s="41"/>
@@ -1492,7 +1496,7 @@
       <c r="L33" s="53"/>
       <c r="M33" s="54">
         <f>(M3-L3)+(M4-L4)+(M5-L5)+(M6-L6)+(M7-L7)+(M8-L8)+(M9-L9)+(M10-L10)+(M11-L11)+(M12-L12)+(M13-L13)+(M14-L14)+(M15-L15)+(M16-L16)</f>
-        <v>0.67638888888888893</v>
+        <v>0.82222222222222219</v>
       </c>
     </row>
     <row r="34" spans="11:13" ht="14.25" customHeight="1">

</xml_diff>